<commit_message>
The serial number for the ADCPA-m for glider deployment 383_00001 was wrong in the calibration sheets.  This commit corrects it.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL383/Omaha_Cal_Info_CE05MOAS-GL383_00001.xlsx
+++ b/CE05MOAS-GL383/Omaha_Cal_Info_CE05MOAS-GL383_00001.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ooi\ingestion-csvs\CE05MOAS-GL383\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="377"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="377" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$77</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$319</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -439,6 +444,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -486,7 +494,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,7 +529,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -732,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -836,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="15">
-        <v>650865</v>
+        <v>649982</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>26</v>
@@ -1062,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="15">
-        <v>650865</v>
+        <v>649982</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>27</v>
@@ -1092,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="15">
-        <v>650865</v>
+        <v>649982</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>28</v>
@@ -1122,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="15">
-        <v>650865</v>
+        <v>649982</v>
       </c>
       <c r="E12" s="22" t="s">
         <v>29</v>

</xml_diff>